<commit_message>
Add Dynamic GANTT tool
</commit_message>
<xml_diff>
--- a/tools/decision_maker/sfDecisionMaking.xlsx
+++ b/tools/decision_maker/sfDecisionMaking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B4CDF9-3EAB-4646-80B6-0BA708ECD643}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178BE3DF-DBA0-4DF7-B001-774D4FFD643D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-195" yWindow="-195" windowWidth="29190" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HowTo" sheetId="20" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -907,7 +907,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -993,16 +993,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>387804</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25173</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>40822</xdr:rowOff>
+      <xdr:rowOff>59192</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>215333</xdr:colOff>
+      <xdr:colOff>505845</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>326572</xdr:rowOff>
+      <xdr:rowOff>344942</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1031,8 +1031,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5558518" y="40822"/>
-          <a:ext cx="1120208" cy="285750"/>
+          <a:off x="5903459" y="59192"/>
+          <a:ext cx="1133815" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1067,8 +1067,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="619126" y="796018"/>
-          <a:ext cx="9041945" cy="3280277"/>
+          <a:off x="619126" y="789214"/>
+          <a:ext cx="9141957" cy="3178224"/>
           <a:chOff x="619126" y="796018"/>
           <a:chExt cx="9041945" cy="3280277"/>
         </a:xfrm>
@@ -1427,8 +1427,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="636815" y="4716237"/>
-          <a:ext cx="5819774" cy="2760888"/>
+          <a:off x="636815" y="4580166"/>
+          <a:ext cx="5881006" cy="2663595"/>
           <a:chOff x="636815" y="4716237"/>
           <a:chExt cx="5819774" cy="2760888"/>
         </a:xfrm>
@@ -1904,8 +1904,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="644978" y="8053022"/>
-          <a:ext cx="9293678" cy="3479031"/>
+          <a:off x="649740" y="7799248"/>
+          <a:ext cx="9395731" cy="3345000"/>
           <a:chOff x="644978" y="8053022"/>
           <a:chExt cx="9293678" cy="3479031"/>
         </a:xfrm>
@@ -2622,7 +2622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742C2AD9-D22B-45FA-9768-B17049A28C1F}">
   <dimension ref="A1:AC57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC41" sqref="AC41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -2897,10 +2899,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:24">
+    <row r="33" spans="2:27">
       <c r="Q33" s="12"/>
     </row>
-    <row r="34" spans="2:24">
+    <row r="34" spans="2:27">
       <c r="Q34" s="12">
         <v>3</v>
       </c>
@@ -2908,7 +2910,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:24">
+    <row r="36" spans="2:27">
       <c r="Q36" s="12">
         <v>4</v>
       </c>
@@ -2916,12 +2918,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:24">
+    <row r="41" spans="2:27">
       <c r="Q41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="2:24">
+    <row r="42" spans="2:27">
       <c r="B42" s="60" t="s">
         <v>56</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="2:24">
+    <row r="45" spans="2:27">
       <c r="Q45" s="62" t="s">
         <v>62</v>
       </c>
@@ -2953,8 +2955,11 @@
       <c r="V45" s="64"/>
       <c r="W45" s="64"/>
       <c r="X45" s="64"/>
-    </row>
-    <row r="46" spans="2:24">
+      <c r="Y45" s="64"/>
+      <c r="Z45" s="64"/>
+      <c r="AA45" s="64"/>
+    </row>
+    <row r="46" spans="2:27">
       <c r="Q46" s="62" t="s">
         <v>63</v>
       </c>
@@ -2965,8 +2970,11 @@
       <c r="V46" s="64"/>
       <c r="W46" s="64"/>
       <c r="X46" s="64"/>
-    </row>
-    <row r="47" spans="2:24">
+      <c r="Y46" s="64"/>
+      <c r="Z46" s="64"/>
+      <c r="AA46" s="64"/>
+    </row>
+    <row r="47" spans="2:27">
       <c r="Q47" s="62" t="s">
         <v>64</v>
       </c>
@@ -2977,8 +2985,11 @@
       <c r="V47" s="64"/>
       <c r="W47" s="64"/>
       <c r="X47" s="64"/>
-    </row>
-    <row r="48" spans="2:24">
+      <c r="Y47" s="64"/>
+      <c r="Z47" s="64"/>
+      <c r="AA47" s="64"/>
+    </row>
+    <row r="48" spans="2:27">
       <c r="Q48" s="62" t="s">
         <v>65</v>
       </c>
@@ -2989,8 +3000,11 @@
       <c r="V48" s="64"/>
       <c r="W48" s="64"/>
       <c r="X48" s="64"/>
-    </row>
-    <row r="49" spans="17:24">
+      <c r="Y48" s="64"/>
+      <c r="Z48" s="64"/>
+      <c r="AA48" s="64"/>
+    </row>
+    <row r="49" spans="17:27">
       <c r="Q49" s="62"/>
       <c r="R49" s="62"/>
       <c r="S49" s="64"/>
@@ -2999,8 +3013,11 @@
       <c r="V49" s="64"/>
       <c r="W49" s="64"/>
       <c r="X49" s="64"/>
-    </row>
-    <row r="50" spans="17:24">
+      <c r="Y49" s="64"/>
+      <c r="Z49" s="64"/>
+      <c r="AA49" s="64"/>
+    </row>
+    <row r="50" spans="17:27">
       <c r="Q50" s="62" t="s">
         <v>66</v>
       </c>
@@ -3011,8 +3028,11 @@
       <c r="V50" s="64"/>
       <c r="W50" s="64"/>
       <c r="X50" s="64"/>
-    </row>
-    <row r="51" spans="17:24">
+      <c r="Y50" s="64"/>
+      <c r="Z50" s="64"/>
+      <c r="AA50" s="64"/>
+    </row>
+    <row r="51" spans="17:27">
       <c r="Q51" s="62" t="s">
         <v>67</v>
       </c>
@@ -3023,8 +3043,11 @@
       <c r="V51" s="64"/>
       <c r="W51" s="64"/>
       <c r="X51" s="64"/>
-    </row>
-    <row r="52" spans="17:24">
+      <c r="Y51" s="64"/>
+      <c r="Z51" s="64"/>
+      <c r="AA51" s="64"/>
+    </row>
+    <row r="52" spans="17:27">
       <c r="Q52" s="62" t="s">
         <v>68</v>
       </c>
@@ -3035,8 +3058,11 @@
       <c r="V52" s="64"/>
       <c r="W52" s="64"/>
       <c r="X52" s="64"/>
-    </row>
-    <row r="53" spans="17:24">
+      <c r="Y52" s="64"/>
+      <c r="Z52" s="64"/>
+      <c r="AA52" s="64"/>
+    </row>
+    <row r="53" spans="17:27">
       <c r="Q53" s="62" t="s">
         <v>69</v>
       </c>
@@ -3047,8 +3073,11 @@
       <c r="V53" s="64"/>
       <c r="W53" s="64"/>
       <c r="X53" s="64"/>
-    </row>
-    <row r="54" spans="17:24">
+      <c r="Y53" s="64"/>
+      <c r="Z53" s="64"/>
+      <c r="AA53" s="64"/>
+    </row>
+    <row r="54" spans="17:27">
       <c r="Q54" s="62"/>
       <c r="R54" s="62"/>
       <c r="S54" s="64"/>
@@ -3057,8 +3086,11 @@
       <c r="V54" s="64"/>
       <c r="W54" s="64"/>
       <c r="X54" s="64"/>
-    </row>
-    <row r="55" spans="17:24">
+      <c r="Y54" s="64"/>
+      <c r="Z54" s="64"/>
+      <c r="AA54" s="64"/>
+    </row>
+    <row r="55" spans="17:27">
       <c r="Q55" s="62" t="s">
         <v>70</v>
       </c>
@@ -3069,8 +3101,11 @@
       <c r="V55" s="64"/>
       <c r="W55" s="64"/>
       <c r="X55" s="64"/>
-    </row>
-    <row r="56" spans="17:24">
+      <c r="Y55" s="64"/>
+      <c r="Z55" s="64"/>
+      <c r="AA55" s="64"/>
+    </row>
+    <row r="56" spans="17:27">
       <c r="Q56" s="62" t="s">
         <v>71</v>
       </c>
@@ -3081,8 +3116,11 @@
       <c r="V56" s="64"/>
       <c r="W56" s="64"/>
       <c r="X56" s="64"/>
-    </row>
-    <row r="57" spans="17:24">
+      <c r="Y56" s="64"/>
+      <c r="Z56" s="64"/>
+      <c r="AA56" s="64"/>
+    </row>
+    <row r="57" spans="17:27">
       <c r="Q57" s="63" t="s">
         <v>72</v>
       </c>
@@ -3093,6 +3131,9 @@
       <c r="V57" s="64"/>
       <c r="W57" s="64"/>
       <c r="X57" s="64"/>
+      <c r="Y57" s="64"/>
+      <c r="Z57" s="64"/>
+      <c r="AA57" s="64"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3637,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="41">
-        <f t="shared" ref="C6:I16" ca="1" si="0">INDIRECT($B6 &amp; "!B" &amp; COLUMN(D6)-1)</f>
+        <f t="shared" ref="C6:I10" ca="1" si="0">INDIRECT($B6 &amp; "!B" &amp; COLUMN(D6)-1)</f>
         <v>5</v>
       </c>
       <c r="E6" s="41">
@@ -3665,11 +3706,11 @@
         <v>2.8125</v>
       </c>
       <c r="K6" s="49">
-        <f ca="1">RANK(J6,J:J,0)</f>
+        <f t="shared" ref="K6:K19" ca="1" si="2">RANK(J6,J:J,0)</f>
         <v>5</v>
       </c>
       <c r="L6" s="48" t="str">
-        <f ca="1">IF(K6&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ref="L6:L37" ca="1" si="3">IF(K6&lt;=$G$1,"Go!","No Go")</f>
         <v>No Go</v>
       </c>
       <c r="M6" s="23"/>
@@ -3681,7 +3722,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="8">
-        <f t="shared" ref="A7:A70" si="2">ROW(B7)-ROW($A$5)</f>
+        <f t="shared" ref="A7:A70" si="4">ROW(B7)-ROW($A$5)</f>
         <v>2</v>
       </c>
       <c r="B7" s="38" t="s">
@@ -3720,11 +3761,11 @@
         <v>3.7321428571428572</v>
       </c>
       <c r="K7" s="49">
-        <f ca="1">RANK(J7,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>3</v>
       </c>
       <c r="L7" s="48" t="str">
-        <f ca="1">IF(K7&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Go!</v>
       </c>
       <c r="M7" s="23"/>
@@ -3736,7 +3777,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -3775,11 +3816,11 @@
         <v>3.9799107142857135</v>
       </c>
       <c r="K8" s="49">
-        <f ca="1">RANK(J8,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
       <c r="L8" s="48" t="str">
-        <f ca="1">IF(K8&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Go!</v>
       </c>
       <c r="M8" s="23"/>
@@ -3791,7 +3832,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="B9" s="38" t="s">
@@ -3830,11 +3871,11 @@
         <v>4.1651785714285712</v>
       </c>
       <c r="K9" s="49">
-        <f ca="1">RANK(J9,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="L9" s="48" t="str">
-        <f ca="1">IF(K9&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>Go!</v>
       </c>
       <c r="M9" s="23"/>
@@ -3846,7 +3887,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B10" s="38" t="s">
@@ -3881,15 +3922,15 @@
         <v>2</v>
       </c>
       <c r="J10" s="22">
-        <f t="shared" ref="J10" ca="1" si="3">(C10*$C$5+D10*$D$5+E10*$E$5+F10*$F$5+G10*$G$5+H10*$H$5+I10*$I$5)</f>
+        <f t="shared" ref="J10" ca="1" si="5">(C10*$C$5+D10*$D$5+E10*$E$5+F10*$F$5+G10*$G$5+H10*$H$5+I10*$I$5)</f>
         <v>3.3236607142857144</v>
       </c>
       <c r="K10" s="49">
-        <f ca="1">RANK(J10,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="L10" s="48" t="str">
-        <f ca="1">IF(K10&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M10" s="23"/>
@@ -3901,7 +3942,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B11" s="46"/>
@@ -3917,11 +3958,11 @@
         <v>0</v>
       </c>
       <c r="K11" s="49">
-        <f ca="1">RANK(J11,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L11" s="48" t="str">
-        <f ca="1">IF(K11&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M11" s="23"/>
@@ -3933,7 +3974,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="B12" s="38"/>
@@ -3949,11 +3990,11 @@
         <v>0</v>
       </c>
       <c r="K12" s="49">
-        <f ca="1">RANK(J12,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L12" s="48" t="str">
-        <f ca="1">IF(K12&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M12" s="23"/>
@@ -3965,7 +4006,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="B13" s="38"/>
@@ -3981,11 +4022,11 @@
         <v>0</v>
       </c>
       <c r="K13" s="49">
-        <f ca="1">RANK(J13,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L13" s="48" t="str">
-        <f ca="1">IF(K13&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M13" s="23"/>
@@ -3997,7 +4038,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="B14" s="38"/>
@@ -4013,11 +4054,11 @@
         <v>0</v>
       </c>
       <c r="K14" s="49">
-        <f ca="1">RANK(J14,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L14" s="48" t="str">
-        <f ca="1">IF(K14&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M14" s="23"/>
@@ -4029,7 +4070,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="B15" s="38"/>
@@ -4045,11 +4086,11 @@
         <v>0</v>
       </c>
       <c r="K15" s="49">
-        <f ca="1">RANK(J15,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L15" s="48" t="str">
-        <f ca="1">IF(K15&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M15" s="23"/>
@@ -4061,7 +4102,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="B16" s="38"/>
@@ -4077,11 +4118,11 @@
         <v>0</v>
       </c>
       <c r="K16" s="49">
-        <f ca="1">RANK(J16,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L16" s="48" t="str">
-        <f ca="1">IF(K16&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M16" s="23"/>
@@ -4093,7 +4134,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="B17" s="38"/>
@@ -4109,11 +4150,11 @@
         <v>0</v>
       </c>
       <c r="K17" s="49">
-        <f ca="1">RANK(J17,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L17" s="48" t="str">
-        <f ca="1">IF(K17&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M17" s="23"/>
@@ -4125,7 +4166,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="B18" s="38"/>
@@ -4141,11 +4182,11 @@
         <v>0</v>
       </c>
       <c r="K18" s="49">
-        <f ca="1">RANK(J18,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L18" s="48" t="str">
-        <f ca="1">IF(K18&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M18" s="23"/>
@@ -4157,7 +4198,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="B19" s="38"/>
@@ -4173,11 +4214,11 @@
         <v>0</v>
       </c>
       <c r="K19" s="49">
-        <f ca="1">RANK(J19,J:J,0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="L19" s="48" t="str">
-        <f ca="1">IF(K19&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M19" s="23"/>
@@ -4189,7 +4230,7 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="B20" s="38"/>
@@ -4205,11 +4246,11 @@
         <v>0</v>
       </c>
       <c r="K20" s="49">
-        <f t="shared" ref="K20:K83" ca="1" si="4">RANK(J20,J:J,0)</f>
+        <f t="shared" ref="K20:K83" ca="1" si="6">RANK(J20,J:J,0)</f>
         <v>6</v>
       </c>
       <c r="L20" s="48" t="str">
-        <f ca="1">IF(K20&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M20" s="23"/>
@@ -4221,7 +4262,7 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="B21" s="38"/>
@@ -4237,11 +4278,11 @@
         <v>0</v>
       </c>
       <c r="K21" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L21" s="48" t="str">
-        <f ca="1">IF(K21&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M21" s="23"/>
@@ -4253,7 +4294,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="B22" s="38"/>
@@ -4269,11 +4310,11 @@
         <v>0</v>
       </c>
       <c r="K22" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L22" s="48" t="str">
-        <f ca="1">IF(K22&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M22" s="23"/>
@@ -4285,7 +4326,7 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="B23" s="38"/>
@@ -4301,11 +4342,11 @@
         <v>0</v>
       </c>
       <c r="K23" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L23" s="48" t="str">
-        <f ca="1">IF(K23&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M23" s="23"/>
@@ -4317,7 +4358,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="B24" s="38"/>
@@ -4333,11 +4374,11 @@
         <v>0</v>
       </c>
       <c r="K24" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L24" s="48" t="str">
-        <f ca="1">IF(K24&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M24" s="23"/>
@@ -4349,7 +4390,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="B25" s="38"/>
@@ -4365,11 +4406,11 @@
         <v>0</v>
       </c>
       <c r="K25" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L25" s="48" t="str">
-        <f ca="1">IF(K25&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M25" s="23"/>
@@ -4381,7 +4422,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="B26" s="47"/>
@@ -4397,11 +4438,11 @@
         <v>0</v>
       </c>
       <c r="K26" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L26" s="48" t="str">
-        <f ca="1">IF(K26&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M26" s="23"/>
@@ -4413,7 +4454,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="B27" s="47"/>
@@ -4429,11 +4470,11 @@
         <v>0</v>
       </c>
       <c r="K27" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L27" s="48" t="str">
-        <f ca="1">IF(K27&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M27" s="23"/>
@@ -4445,7 +4486,7 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="B28" s="47"/>
@@ -4461,11 +4502,11 @@
         <v>0</v>
       </c>
       <c r="K28" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L28" s="48" t="str">
-        <f ca="1">IF(K28&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M28" s="23"/>
@@ -4477,7 +4518,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="B29" s="47"/>
@@ -4493,11 +4534,11 @@
         <v>0</v>
       </c>
       <c r="K29" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L29" s="48" t="str">
-        <f ca="1">IF(K29&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M29" s="23"/>
@@ -4509,7 +4550,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B30" s="47"/>
@@ -4525,11 +4566,11 @@
         <v>0</v>
       </c>
       <c r="K30" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L30" s="48" t="str">
-        <f ca="1">IF(K30&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M30" s="23"/>
@@ -4541,7 +4582,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="B31" s="47"/>
@@ -4557,11 +4598,11 @@
         <v>0</v>
       </c>
       <c r="K31" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L31" s="48" t="str">
-        <f ca="1">IF(K31&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M31" s="23"/>
@@ -4573,7 +4614,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="B32" s="47"/>
@@ -4589,11 +4630,11 @@
         <v>0</v>
       </c>
       <c r="K32" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L32" s="48" t="str">
-        <f ca="1">IF(K32&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M32" s="23"/>
@@ -4605,7 +4646,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="B33" s="47"/>
@@ -4621,11 +4662,11 @@
         <v>0</v>
       </c>
       <c r="K33" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L33" s="48" t="str">
-        <f ca="1">IF(K33&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M33" s="23"/>
@@ -4637,7 +4678,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="B34" s="47"/>
@@ -4653,11 +4694,11 @@
         <v>0</v>
       </c>
       <c r="K34" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L34" s="48" t="str">
-        <f ca="1">IF(K34&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M34" s="23"/>
@@ -4669,7 +4710,7 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="B35" s="47"/>
@@ -4685,11 +4726,11 @@
         <v>0</v>
       </c>
       <c r="K35" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L35" s="48" t="str">
-        <f ca="1">IF(K35&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M35" s="23"/>
@@ -4701,7 +4742,7 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="B36" s="47"/>
@@ -4717,11 +4758,11 @@
         <v>0</v>
       </c>
       <c r="K36" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L36" s="48" t="str">
-        <f ca="1">IF(K36&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M36" s="23"/>
@@ -4733,7 +4774,7 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="B37" s="47"/>
@@ -4749,11 +4790,11 @@
         <v>0</v>
       </c>
       <c r="K37" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L37" s="48" t="str">
-        <f ca="1">IF(K37&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="3"/>
         <v>No Go</v>
       </c>
       <c r="M37" s="23"/>
@@ -4765,7 +4806,7 @@
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="B38" s="47"/>
@@ -4781,11 +4822,11 @@
         <v>0</v>
       </c>
       <c r="K38" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L38" s="48" t="str">
-        <f ca="1">IF(K38&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ref="L38:L69" ca="1" si="7">IF(K38&lt;=$G$1,"Go!","No Go")</f>
         <v>No Go</v>
       </c>
       <c r="M38" s="23"/>
@@ -4797,7 +4838,7 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="B39" s="47"/>
@@ -4813,11 +4854,11 @@
         <v>0</v>
       </c>
       <c r="K39" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L39" s="48" t="str">
-        <f ca="1">IF(K39&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M39" s="23"/>
@@ -4829,7 +4870,7 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="B40" s="47"/>
@@ -4845,11 +4886,11 @@
         <v>0</v>
       </c>
       <c r="K40" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L40" s="48" t="str">
-        <f ca="1">IF(K40&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M40" s="23"/>
@@ -4861,7 +4902,7 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="B41" s="47"/>
@@ -4877,11 +4918,11 @@
         <v>0</v>
       </c>
       <c r="K41" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L41" s="48" t="str">
-        <f ca="1">IF(K41&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M41" s="23"/>
@@ -4893,7 +4934,7 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="B42" s="47"/>
@@ -4909,11 +4950,11 @@
         <v>0</v>
       </c>
       <c r="K42" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L42" s="48" t="str">
-        <f ca="1">IF(K42&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M42" s="23"/>
@@ -4925,7 +4966,7 @@
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
       <c r="B43" s="47"/>
@@ -4941,11 +4982,11 @@
         <v>0</v>
       </c>
       <c r="K43" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L43" s="48" t="str">
-        <f ca="1">IF(K43&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M43" s="23"/>
@@ -4957,7 +4998,7 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="B44" s="47"/>
@@ -4973,11 +5014,11 @@
         <v>0</v>
       </c>
       <c r="K44" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L44" s="48" t="str">
-        <f ca="1">IF(K44&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M44" s="23"/>
@@ -4989,7 +5030,7 @@
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="B45" s="47"/>
@@ -5005,11 +5046,11 @@
         <v>0</v>
       </c>
       <c r="K45" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L45" s="48" t="str">
-        <f ca="1">IF(K45&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M45" s="23"/>
@@ -5021,7 +5062,7 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="B46" s="47"/>
@@ -5037,11 +5078,11 @@
         <v>0</v>
       </c>
       <c r="K46" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L46" s="48" t="str">
-        <f ca="1">IF(K46&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M46" s="23"/>
@@ -5053,7 +5094,7 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="B47" s="47"/>
@@ -5069,11 +5110,11 @@
         <v>0</v>
       </c>
       <c r="K47" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L47" s="48" t="str">
-        <f ca="1">IF(K47&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M47" s="23"/>
@@ -5085,7 +5126,7 @@
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="B48" s="47"/>
@@ -5101,11 +5142,11 @@
         <v>0</v>
       </c>
       <c r="K48" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L48" s="48" t="str">
-        <f ca="1">IF(K48&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M48" s="23"/>
@@ -5117,7 +5158,7 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="B49" s="47"/>
@@ -5133,11 +5174,11 @@
         <v>0</v>
       </c>
       <c r="K49" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L49" s="48" t="str">
-        <f ca="1">IF(K49&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M49" s="23"/>
@@ -5149,7 +5190,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="B50" s="47"/>
@@ -5165,11 +5206,11 @@
         <v>0</v>
       </c>
       <c r="K50" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L50" s="48" t="str">
-        <f ca="1">IF(K50&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M50" s="23"/>
@@ -5181,7 +5222,7 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="B51" s="47"/>
@@ -5197,11 +5238,11 @@
         <v>0</v>
       </c>
       <c r="K51" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L51" s="48" t="str">
-        <f ca="1">IF(K51&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M51" s="23"/>
@@ -5213,7 +5254,7 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="B52" s="47"/>
@@ -5229,11 +5270,11 @@
         <v>0</v>
       </c>
       <c r="K52" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L52" s="48" t="str">
-        <f ca="1">IF(K52&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M52" s="23"/>
@@ -5245,7 +5286,7 @@
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="B53" s="47"/>
@@ -5261,11 +5302,11 @@
         <v>0</v>
       </c>
       <c r="K53" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L53" s="48" t="str">
-        <f ca="1">IF(K53&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M53" s="23"/>
@@ -5277,7 +5318,7 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="B54" s="47"/>
@@ -5293,11 +5334,11 @@
         <v>0</v>
       </c>
       <c r="K54" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L54" s="48" t="str">
-        <f ca="1">IF(K54&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M54" s="23"/>
@@ -5309,7 +5350,7 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="B55" s="47"/>
@@ -5325,11 +5366,11 @@
         <v>0</v>
       </c>
       <c r="K55" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L55" s="48" t="str">
-        <f ca="1">IF(K55&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M55" s="23"/>
@@ -5341,7 +5382,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="B56" s="47"/>
@@ -5357,11 +5398,11 @@
         <v>0</v>
       </c>
       <c r="K56" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L56" s="48" t="str">
-        <f ca="1">IF(K56&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M56" s="23"/>
@@ -5373,7 +5414,7 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="B57" s="47"/>
@@ -5389,11 +5430,11 @@
         <v>0</v>
       </c>
       <c r="K57" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L57" s="48" t="str">
-        <f ca="1">IF(K57&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M57" s="23"/>
@@ -5405,7 +5446,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="B58" s="47"/>
@@ -5421,11 +5462,11 @@
         <v>0</v>
       </c>
       <c r="K58" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L58" s="48" t="str">
-        <f ca="1">IF(K58&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M58" s="23"/>
@@ -5437,7 +5478,7 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="B59" s="47"/>
@@ -5453,11 +5494,11 @@
         <v>0</v>
       </c>
       <c r="K59" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L59" s="48" t="str">
-        <f ca="1">IF(K59&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M59" s="23"/>
@@ -5469,7 +5510,7 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="B60" s="47"/>
@@ -5485,11 +5526,11 @@
         <v>0</v>
       </c>
       <c r="K60" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L60" s="48" t="str">
-        <f ca="1">IF(K60&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M60" s="23"/>
@@ -5501,7 +5542,7 @@
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="B61" s="47"/>
@@ -5517,11 +5558,11 @@
         <v>0</v>
       </c>
       <c r="K61" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L61" s="48" t="str">
-        <f ca="1">IF(K61&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M61" s="23"/>
@@ -5533,7 +5574,7 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="B62" s="47"/>
@@ -5549,11 +5590,11 @@
         <v>0</v>
       </c>
       <c r="K62" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L62" s="48" t="str">
-        <f ca="1">IF(K62&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M62" s="23"/>
@@ -5565,7 +5606,7 @@
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="B63" s="47"/>
@@ -5581,11 +5622,11 @@
         <v>0</v>
       </c>
       <c r="K63" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L63" s="48" t="str">
-        <f ca="1">IF(K63&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M63" s="23"/>
@@ -5597,7 +5638,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="B64" s="47"/>
@@ -5613,11 +5654,11 @@
         <v>0</v>
       </c>
       <c r="K64" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L64" s="48" t="str">
-        <f ca="1">IF(K64&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M64" s="23"/>
@@ -5629,7 +5670,7 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="B65" s="47"/>
@@ -5645,11 +5686,11 @@
         <v>0</v>
       </c>
       <c r="K65" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L65" s="48" t="str">
-        <f ca="1">IF(K65&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M65" s="23"/>
@@ -5661,7 +5702,7 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="B66" s="47"/>
@@ -5677,11 +5718,11 @@
         <v>0</v>
       </c>
       <c r="K66" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L66" s="48" t="str">
-        <f ca="1">IF(K66&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M66" s="23"/>
@@ -5693,7 +5734,7 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="B67" s="47"/>
@@ -5709,11 +5750,11 @@
         <v>0</v>
       </c>
       <c r="K67" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L67" s="48" t="str">
-        <f ca="1">IF(K67&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M67" s="23"/>
@@ -5725,7 +5766,7 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="B68" s="47"/>
@@ -5741,11 +5782,11 @@
         <v>0</v>
       </c>
       <c r="K68" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L68" s="48" t="str">
-        <f ca="1">IF(K68&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M68" s="23"/>
@@ -5757,7 +5798,7 @@
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="B69" s="47"/>
@@ -5773,11 +5814,11 @@
         <v>0</v>
       </c>
       <c r="K69" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L69" s="48" t="str">
-        <f ca="1">IF(K69&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="7"/>
         <v>No Go</v>
       </c>
       <c r="M69" s="23"/>
@@ -5789,7 +5830,7 @@
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="B70" s="47"/>
@@ -5801,15 +5842,15 @@
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="22">
-        <f t="shared" ref="J70:J105" si="5">(C70*$C$5+D70*$D$5+E70*$E$5+F70*$F$5+G70*$G$5+H70*$H$5+I70*$I$5)</f>
+        <f t="shared" ref="J70:J105" si="8">(C70*$C$5+D70*$D$5+E70*$E$5+F70*$F$5+G70*$G$5+H70*$H$5+I70*$I$5)</f>
         <v>0</v>
       </c>
       <c r="K70" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L70" s="48" t="str">
-        <f ca="1">IF(K70&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ref="L70:L101" ca="1" si="9">IF(K70&lt;=$G$1,"Go!","No Go")</f>
         <v>No Go</v>
       </c>
       <c r="M70" s="23"/>
@@ -5821,7 +5862,7 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="8">
-        <f t="shared" ref="A71:A105" si="6">ROW(B71)-ROW($A$5)</f>
+        <f t="shared" ref="A71:A105" si="10">ROW(B71)-ROW($A$5)</f>
         <v>66</v>
       </c>
       <c r="B71" s="47"/>
@@ -5833,15 +5874,15 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K71" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L71" s="48" t="str">
-        <f ca="1">IF(K71&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M71" s="23"/>
@@ -5853,7 +5894,7 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>67</v>
       </c>
       <c r="B72" s="47"/>
@@ -5865,15 +5906,15 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
       <c r="J72" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K72" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L72" s="48" t="str">
-        <f ca="1">IF(K72&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M72" s="23"/>
@@ -5885,7 +5926,7 @@
     </row>
     <row r="73" spans="1:18">
       <c r="A73" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>68</v>
       </c>
       <c r="B73" s="47"/>
@@ -5897,15 +5938,15 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
       <c r="J73" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K73" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L73" s="48" t="str">
-        <f ca="1">IF(K73&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M73" s="23"/>
@@ -5917,7 +5958,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>69</v>
       </c>
       <c r="B74" s="47"/>
@@ -5929,15 +5970,15 @@
       <c r="H74" s="20"/>
       <c r="I74" s="20"/>
       <c r="J74" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K74" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L74" s="48" t="str">
-        <f ca="1">IF(K74&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M74" s="23"/>
@@ -5949,7 +5990,7 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="B75" s="47"/>
@@ -5961,15 +6002,15 @@
       <c r="H75" s="20"/>
       <c r="I75" s="20"/>
       <c r="J75" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K75" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L75" s="48" t="str">
-        <f ca="1">IF(K75&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M75" s="23"/>
@@ -5981,7 +6022,7 @@
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>71</v>
       </c>
       <c r="B76" s="47"/>
@@ -5993,15 +6034,15 @@
       <c r="H76" s="20"/>
       <c r="I76" s="20"/>
       <c r="J76" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K76" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L76" s="48" t="str">
-        <f ca="1">IF(K76&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M76" s="23"/>
@@ -6013,7 +6054,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
       <c r="B77" s="47"/>
@@ -6025,15 +6066,15 @@
       <c r="H77" s="20"/>
       <c r="I77" s="20"/>
       <c r="J77" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K77" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L77" s="48" t="str">
-        <f ca="1">IF(K77&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M77" s="23"/>
@@ -6045,7 +6086,7 @@
     </row>
     <row r="78" spans="1:18">
       <c r="A78" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>73</v>
       </c>
       <c r="B78" s="47"/>
@@ -6057,15 +6098,15 @@
       <c r="H78" s="20"/>
       <c r="I78" s="20"/>
       <c r="J78" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K78" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L78" s="48" t="str">
-        <f ca="1">IF(K78&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M78" s="23"/>
@@ -6077,7 +6118,7 @@
     </row>
     <row r="79" spans="1:18">
       <c r="A79" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>74</v>
       </c>
       <c r="B79" s="47"/>
@@ -6089,15 +6130,15 @@
       <c r="H79" s="20"/>
       <c r="I79" s="20"/>
       <c r="J79" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K79" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L79" s="48" t="str">
-        <f ca="1">IF(K79&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M79" s="23"/>
@@ -6109,7 +6150,7 @@
     </row>
     <row r="80" spans="1:18">
       <c r="A80" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>75</v>
       </c>
       <c r="B80" s="47"/>
@@ -6121,15 +6162,15 @@
       <c r="H80" s="20"/>
       <c r="I80" s="20"/>
       <c r="J80" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K80" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L80" s="48" t="str">
-        <f ca="1">IF(K80&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M80" s="23"/>
@@ -6141,7 +6182,7 @@
     </row>
     <row r="81" spans="1:18">
       <c r="A81" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>76</v>
       </c>
       <c r="B81" s="47"/>
@@ -6153,15 +6194,15 @@
       <c r="H81" s="20"/>
       <c r="I81" s="20"/>
       <c r="J81" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K81" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L81" s="48" t="str">
-        <f ca="1">IF(K81&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M81" s="23"/>
@@ -6173,7 +6214,7 @@
     </row>
     <row r="82" spans="1:18">
       <c r="A82" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>77</v>
       </c>
       <c r="B82" s="47"/>
@@ -6185,15 +6226,15 @@
       <c r="H82" s="20"/>
       <c r="I82" s="20"/>
       <c r="J82" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K82" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L82" s="48" t="str">
-        <f ca="1">IF(K82&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M82" s="23"/>
@@ -6205,7 +6246,7 @@
     </row>
     <row r="83" spans="1:18">
       <c r="A83" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
       <c r="B83" s="47"/>
@@ -6217,15 +6258,15 @@
       <c r="H83" s="20"/>
       <c r="I83" s="20"/>
       <c r="J83" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K83" s="49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
       <c r="L83" s="48" t="str">
-        <f ca="1">IF(K83&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M83" s="23"/>
@@ -6237,7 +6278,7 @@
     </row>
     <row r="84" spans="1:18">
       <c r="A84" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>79</v>
       </c>
       <c r="B84" s="47"/>
@@ -6249,15 +6290,15 @@
       <c r="H84" s="20"/>
       <c r="I84" s="20"/>
       <c r="J84" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K84" s="49">
-        <f t="shared" ref="K84:K105" ca="1" si="7">RANK(J84,J:J,0)</f>
+        <f t="shared" ref="K84:K105" ca="1" si="11">RANK(J84,J:J,0)</f>
         <v>6</v>
       </c>
       <c r="L84" s="48" t="str">
-        <f ca="1">IF(K84&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M84" s="23"/>
@@ -6269,7 +6310,7 @@
     </row>
     <row r="85" spans="1:18">
       <c r="A85" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="B85" s="47"/>
@@ -6281,15 +6322,15 @@
       <c r="H85" s="20"/>
       <c r="I85" s="20"/>
       <c r="J85" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K85" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L85" s="48" t="str">
-        <f ca="1">IF(K85&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M85" s="23"/>
@@ -6301,7 +6342,7 @@
     </row>
     <row r="86" spans="1:18">
       <c r="A86" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>81</v>
       </c>
       <c r="B86" s="47"/>
@@ -6313,15 +6354,15 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
       <c r="J86" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K86" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L86" s="48" t="str">
-        <f ca="1">IF(K86&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M86" s="23"/>
@@ -6333,7 +6374,7 @@
     </row>
     <row r="87" spans="1:18">
       <c r="A87" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>82</v>
       </c>
       <c r="B87" s="47"/>
@@ -6345,15 +6386,15 @@
       <c r="H87" s="20"/>
       <c r="I87" s="20"/>
       <c r="J87" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K87" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L87" s="48" t="str">
-        <f ca="1">IF(K87&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M87" s="23"/>
@@ -6365,7 +6406,7 @@
     </row>
     <row r="88" spans="1:18">
       <c r="A88" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>83</v>
       </c>
       <c r="B88" s="47"/>
@@ -6377,15 +6418,15 @@
       <c r="H88" s="20"/>
       <c r="I88" s="20"/>
       <c r="J88" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K88" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L88" s="48" t="str">
-        <f ca="1">IF(K88&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M88" s="23"/>
@@ -6397,7 +6438,7 @@
     </row>
     <row r="89" spans="1:18">
       <c r="A89" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>84</v>
       </c>
       <c r="B89" s="47"/>
@@ -6409,15 +6450,15 @@
       <c r="H89" s="20"/>
       <c r="I89" s="20"/>
       <c r="J89" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K89" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L89" s="48" t="str">
-        <f ca="1">IF(K89&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M89" s="23"/>
@@ -6429,7 +6470,7 @@
     </row>
     <row r="90" spans="1:18">
       <c r="A90" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>85</v>
       </c>
       <c r="B90" s="47"/>
@@ -6441,15 +6482,15 @@
       <c r="H90" s="20"/>
       <c r="I90" s="20"/>
       <c r="J90" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K90" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L90" s="48" t="str">
-        <f ca="1">IF(K90&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M90" s="23"/>
@@ -6461,7 +6502,7 @@
     </row>
     <row r="91" spans="1:18">
       <c r="A91" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>86</v>
       </c>
       <c r="B91" s="47"/>
@@ -6473,15 +6514,15 @@
       <c r="H91" s="20"/>
       <c r="I91" s="20"/>
       <c r="J91" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K91" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L91" s="48" t="str">
-        <f ca="1">IF(K91&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M91" s="23"/>
@@ -6493,7 +6534,7 @@
     </row>
     <row r="92" spans="1:18">
       <c r="A92" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>87</v>
       </c>
       <c r="B92" s="47"/>
@@ -6505,15 +6546,15 @@
       <c r="H92" s="20"/>
       <c r="I92" s="20"/>
       <c r="J92" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K92" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L92" s="48" t="str">
-        <f ca="1">IF(K92&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M92" s="23"/>
@@ -6525,7 +6566,7 @@
     </row>
     <row r="93" spans="1:18">
       <c r="A93" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>88</v>
       </c>
       <c r="B93" s="47"/>
@@ -6537,15 +6578,15 @@
       <c r="H93" s="20"/>
       <c r="I93" s="20"/>
       <c r="J93" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K93" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L93" s="48" t="str">
-        <f ca="1">IF(K93&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M93" s="23"/>
@@ -6557,7 +6598,7 @@
     </row>
     <row r="94" spans="1:18">
       <c r="A94" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>89</v>
       </c>
       <c r="B94" s="47"/>
@@ -6569,15 +6610,15 @@
       <c r="H94" s="20"/>
       <c r="I94" s="20"/>
       <c r="J94" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K94" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L94" s="48" t="str">
-        <f ca="1">IF(K94&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M94" s="23"/>
@@ -6589,7 +6630,7 @@
     </row>
     <row r="95" spans="1:18">
       <c r="A95" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="B95" s="47"/>
@@ -6601,15 +6642,15 @@
       <c r="H95" s="20"/>
       <c r="I95" s="20"/>
       <c r="J95" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K95" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L95" s="48" t="str">
-        <f ca="1">IF(K95&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M95" s="23"/>
@@ -6621,7 +6662,7 @@
     </row>
     <row r="96" spans="1:18">
       <c r="A96" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
       <c r="B96" s="47"/>
@@ -6633,15 +6674,15 @@
       <c r="H96" s="20"/>
       <c r="I96" s="20"/>
       <c r="J96" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K96" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L96" s="48" t="str">
-        <f ca="1">IF(K96&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M96" s="23"/>
@@ -6653,7 +6694,7 @@
     </row>
     <row r="97" spans="1:18">
       <c r="A97" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
       <c r="B97" s="47"/>
@@ -6665,15 +6706,15 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
       <c r="J97" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K97" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L97" s="48" t="str">
-        <f ca="1">IF(K97&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M97" s="23"/>
@@ -6685,7 +6726,7 @@
     </row>
     <row r="98" spans="1:18">
       <c r="A98" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>93</v>
       </c>
       <c r="B98" s="47"/>
@@ -6697,15 +6738,15 @@
       <c r="H98" s="20"/>
       <c r="I98" s="20"/>
       <c r="J98" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K98" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L98" s="48" t="str">
-        <f ca="1">IF(K98&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M98" s="23"/>
@@ -6717,7 +6758,7 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>94</v>
       </c>
       <c r="B99" s="47"/>
@@ -6729,15 +6770,15 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
       <c r="J99" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K99" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L99" s="48" t="str">
-        <f ca="1">IF(K99&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M99" s="23"/>
@@ -6749,7 +6790,7 @@
     </row>
     <row r="100" spans="1:18">
       <c r="A100" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>95</v>
       </c>
       <c r="B100" s="47"/>
@@ -6761,15 +6802,15 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
       <c r="J100" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K100" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L100" s="48" t="str">
-        <f ca="1">IF(K100&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M100" s="23"/>
@@ -6781,7 +6822,7 @@
     </row>
     <row r="101" spans="1:18">
       <c r="A101" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>96</v>
       </c>
       <c r="B101" s="47"/>
@@ -6793,15 +6834,15 @@
       <c r="H101" s="20"/>
       <c r="I101" s="20"/>
       <c r="J101" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K101" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L101" s="48" t="str">
-        <f ca="1">IF(K101&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="9"/>
         <v>No Go</v>
       </c>
       <c r="M101" s="23"/>
@@ -6813,7 +6854,7 @@
     </row>
     <row r="102" spans="1:18">
       <c r="A102" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
       <c r="B102" s="47"/>
@@ -6825,15 +6866,15 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
       <c r="J102" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K102" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L102" s="48" t="str">
-        <f ca="1">IF(K102&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ref="L102:L133" ca="1" si="12">IF(K102&lt;=$G$1,"Go!","No Go")</f>
         <v>No Go</v>
       </c>
       <c r="M102" s="23"/>
@@ -6845,7 +6886,7 @@
     </row>
     <row r="103" spans="1:18">
       <c r="A103" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>98</v>
       </c>
       <c r="B103" s="47"/>
@@ -6857,15 +6898,15 @@
       <c r="H103" s="20"/>
       <c r="I103" s="20"/>
       <c r="J103" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K103" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L103" s="48" t="str">
-        <f ca="1">IF(K103&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="12"/>
         <v>No Go</v>
       </c>
       <c r="M103" s="23"/>
@@ -6877,7 +6918,7 @@
     </row>
     <row r="104" spans="1:18">
       <c r="A104" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>99</v>
       </c>
       <c r="B104" s="47"/>
@@ -6889,15 +6930,15 @@
       <c r="H104" s="20"/>
       <c r="I104" s="20"/>
       <c r="J104" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K104" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L104" s="48" t="str">
-        <f ca="1">IF(K104&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="12"/>
         <v>No Go</v>
       </c>
       <c r="M104" s="23"/>
@@ -6909,7 +6950,7 @@
     </row>
     <row r="105" spans="1:18">
       <c r="A105" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="B105" s="47"/>
@@ -6921,15 +6962,15 @@
       <c r="H105" s="20"/>
       <c r="I105" s="20"/>
       <c r="J105" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K105" s="49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="L105" s="48" t="str">
-        <f ca="1">IF(K105&lt;=$G$1,"Go!","No Go")</f>
+        <f t="shared" ca="1" si="12"/>
         <v>No Go</v>
       </c>
       <c r="M105" s="23"/>

</xml_diff>